<commit_message>
Save Draft Version 1
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.number.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.number.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849D3C2A-765A-E545-8962-628B3DE51896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D351F-E28E-7F4A-8A4C-1239879D354A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66140" yWindow="-5560" windowWidth="47080" windowHeight="18220" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="900" yWindow="13820" windowWidth="38400" windowHeight="22620" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-NUMBER" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>code</t>
   </si>
@@ -208,11 +208,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WF.NUM.FILE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WFR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W.File.Request</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyMMdd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`${prefix}${time}${seed}`</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -701,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71967B7B-87F9-4846-9FA6-1A2C9E90AB57}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -988,7 +996,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>50</v>
@@ -997,13 +1005,13 @@
         <v>36</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="6">
@@ -1015,7 +1023,9 @@
       <c r="K9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="M9" s="14"/>
     </row>
   </sheetData>

</xml_diff>